<commit_message>
fix lior double files
</commit_message>
<xml_diff>
--- a/BirdsControl/login_file.xlsx
+++ b/BirdsControl/login_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alter\Desktop\school\Second_Year\Second_semester\testing_and_quallity\BirdsControl\BirdsControl\BirdsControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gofma\OneDrive\שולחן העבודה\BirdsControl\BirdsControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BBE61B-3D98-4CB5-AEEE-B64B01433FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A81C1D-3F17-4045-A84F-5F6B42189218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="18851" windowHeight="9844" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>email</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>lior1234@</t>
-  </si>
-  <si>
-    <t>ritay12</t>
-  </si>
-  <si>
-    <t>ritay12@</t>
   </si>
 </sst>
 </file>
@@ -79,7 +73,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -125,7 +119,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -421,16 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04331750-A4CC-4FB1-9F16-817AAA4C0DCC}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.4140625" customWidth="1"/>
+    <col min="3" max="3" width="20.4140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -543,17 +537,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>311434621</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bugs in chick and in signup
</commit_message>
<xml_diff>
--- a/BirdsControl/login_file.xlsx
+++ b/BirdsControl/login_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gofma\OneDrive\שולחן העבודה\BirdsControl\BirdsControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niron\Desktop\BirdsControl\BirdsControl\BirdsControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A81C1D-3F17-4045-A84F-5F6B42189218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C89A32A-6223-4446-926F-DA422D5879A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>email</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>lior1234@</t>
+  </si>
+  <si>
+    <t>nironi1</t>
   </si>
 </sst>
 </file>
@@ -415,19 +418,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04331750-A4CC-4FB1-9F16-817AAA4C0DCC}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.4140625" customWidth="1"/>
-    <col min="3" max="3" width="20.4140625" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" customWidth="1"/>
+    <col min="3" max="3" width="20.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -449,7 +452,7 @@
         <v>209375906</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -460,7 +463,7 @@
         <v>209375908</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -471,7 +474,7 @@
         <v>209375909</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -482,7 +485,7 @@
         <v>208212191</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -493,7 +496,7 @@
         <v>208212192</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -504,7 +507,7 @@
         <v>209375904</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -515,7 +518,7 @@
         <v>315434621</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -526,7 +529,7 @@
         <v>209375806</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -535,6 +538,17 @@
       </c>
       <c r="C10">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>209375900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test every line to see if crashes
</commit_message>
<xml_diff>
--- a/BirdsControl/login_file.xlsx
+++ b/BirdsControl/login_file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niron\Desktop\BirdsControl\BirdsControl\BirdsControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alter\Desktop\school\Second_Year\Second_semester\testing_and_quallity\BirdsControl\BirdsControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C89A32A-6223-4446-926F-DA422D5879A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E50E92-C908-4F89-B069-7AF1D4D6624B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>nironi1</t>
+  </si>
+  <si>
+    <t>Eitay12</t>
+  </si>
+  <si>
+    <t>Eitay!@12</t>
   </si>
 </sst>
 </file>
@@ -76,7 +82,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -122,7 +128,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -418,19 +424,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04331750-A4CC-4FB1-9F16-817AAA4C0DCC}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.3984375" customWidth="1"/>
-    <col min="3" max="3" width="20.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -452,7 +458,7 @@
         <v>209375906</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -463,7 +469,7 @@
         <v>209375908</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -474,7 +480,7 @@
         <v>209375909</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -485,7 +491,7 @@
         <v>208212191</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -496,7 +502,7 @@
         <v>208212192</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -507,7 +513,7 @@
         <v>209375904</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -518,7 +524,7 @@
         <v>315434621</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -529,7 +535,7 @@
         <v>209375806</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -540,7 +546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -549,6 +555,17 @@
       </c>
       <c r="C11">
         <v>209375900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>314434621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug in sign up fix it
</commit_message>
<xml_diff>
--- a/BirdsControl/login_file.xlsx
+++ b/BirdsControl/login_file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alter\Desktop\school\Second_Year\Second_semester\testing_and_quallity\BirdsControl\BirdsControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niron\Desktop\BirdsControl\BirdsControl\BirdsControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E50E92-C908-4F89-B069-7AF1D4D6624B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D6E4F0-3934-466B-B812-C3762B77F08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{056BD8C1-C541-4C84-A611-2C9B857187B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Eitay!@12</t>
+  </si>
+  <si>
+    <t>niro12</t>
+  </si>
+  <si>
+    <t>nironi1@</t>
   </si>
 </sst>
 </file>
@@ -82,7 +88,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -128,7 +134,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -424,19 +430,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04331750-A4CC-4FB1-9F16-817AAA4C0DCC}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" customWidth="1"/>
+    <col min="3" max="3" width="20.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -458,7 +464,7 @@
         <v>209375906</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -469,7 +475,7 @@
         <v>209375908</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -480,7 +486,7 @@
         <v>209375909</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -491,7 +497,7 @@
         <v>208212191</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -502,7 +508,7 @@
         <v>208212192</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -513,7 +519,7 @@
         <v>209375904</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -524,7 +530,7 @@
         <v>315434621</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -535,7 +541,7 @@
         <v>209375806</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -546,7 +552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -557,7 +563,7 @@
         <v>209375900</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -566,6 +572,17 @@
       </c>
       <c r="C12">
         <v>314434621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>309375905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>